<commit_message>
Room && live mode
</commit_message>
<xml_diff>
--- a/excel/item.xlsx
+++ b/excel/item.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="164">
   <si>
     <t>物品ID</t>
   </si>
@@ -500,6 +500,9 @@
   </si>
   <si>
     <t>豪华宝箱</t>
+  </si>
+  <si>
+    <t>入场劵</t>
   </si>
 </sst>
 </file>
@@ -1938,7 +1941,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:J70"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -3869,6 +3872,26 @@
       <c r="I70" s="19"/>
       <c r="J70" s="19"/>
     </row>
+    <row r="71" ht="13.5" customHeight="1">
+      <c r="A71" s="12">
+        <v>1001</v>
+      </c>
+      <c r="B71" t="s" s="13">
+        <v>163</v>
+      </c>
+      <c r="C71" s="14">
+        <v>8</v>
+      </c>
+      <c r="D71" s="14">
+        <v>999</v>
+      </c>
+      <c r="E71" s="19"/>
+      <c r="F71" s="19"/>
+      <c r="G71" s="19"/>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+      <c r="J71" s="19"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>

</xml_diff>